<commit_message>
Formato de tiempo y totales
</commit_message>
<xml_diff>
--- a/data_example.xlsx
+++ b/data_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anheuserbuschinbev.sharepoint.com/sites/TechSalesSharepoint/Documentos compartidos/Desarrollos/Rutas vendedores/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Company Drive\Anheuser-Busch InBev\Tech Sales Sharepoint - Documentos\Desarrollos\Rutas vendedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{40B198B1-F5DE-439A-9502-66EC0C86AE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A65A623-984B-4403-B45F-D52B582A01B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD86C76-C767-408A-BD77-658864A4631F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8EC8495-D423-46C9-93F1-EC7AA00E2041}"/>
   </bookViews>
@@ -71,19 +71,19 @@
     <t>longitud</t>
   </si>
   <si>
-    <t xml:space="preserve">BAR LEO        </t>
-  </si>
-  <si>
     <t>CENTRO MBARE</t>
   </si>
   <si>
-    <t xml:space="preserve">JORGE GOMEZ                   </t>
-  </si>
-  <si>
     <t>JU</t>
   </si>
   <si>
-    <t xml:space="preserve">COP.TRES HNOS. </t>
+    <t>DESPENSA X</t>
+  </si>
+  <si>
+    <t>NOMBRE VENDEDOR EJEMPLO</t>
+  </si>
+  <si>
+    <t>BODEGA EJEMPLO</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,13 +484,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7</v>
+        <v>8888</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2">
         <v>1101</v>
@@ -499,13 +499,13 @@
         <v>547</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I2">
         <v>-25.278887999999998</v>
@@ -516,13 +516,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>32</v>
+        <v>9999</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>1101</v>
@@ -531,13 +531,13 @@
         <v>547</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I3">
         <v>-25.276754</v>
@@ -552,26 +552,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a89c0d28-3d55-426b-ac2f-beea81b060a8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="49b9c03f-d9b0-4ae5-8c08-7097d6e2ef99" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100446BA24B07D9844DB98058BA4C499492" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="29e676859a0a4878f8d0e52dea794e6f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a89c0d28-3d55-426b-ac2f-beea81b060a8" xmlns:ns3="49b9c03f-d9b0-4ae5-8c08-7097d6e2ef99" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="87590c61fcdddb214fcc01c6e98bb6e4" ns2:_="" ns3:_="">
     <xsd:import namespace="a89c0d28-3d55-426b-ac2f-beea81b060a8"/>
@@ -794,26 +774,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a89c0d28-3d55-426b-ac2f-beea81b060a8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="49b9c03f-d9b0-4ae5-8c08-7097d6e2ef99" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13F15913-018B-4FE6-B184-70222E038F29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a89c0d28-3d55-426b-ac2f-beea81b060a8"/>
-    <ds:schemaRef ds:uri="49b9c03f-d9b0-4ae5-8c08-7097d6e2ef99"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B302C4BA-1653-4DE6-9F96-78B4685ECD3F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47A88FAC-5DC6-4308-B174-5AE45B501F3C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -830,4 +811,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B302C4BA-1653-4DE6-9F96-78B4685ECD3F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13F15913-018B-4FE6-B184-70222E038F29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a89c0d28-3d55-426b-ac2f-beea81b060a8"/>
+    <ds:schemaRef ds:uri="49b9c03f-d9b0-4ae5-8c08-7097d6e2ef99"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>